<commit_message>
add chapter 4 and 5
</commit_message>
<xml_diff>
--- a/Data/house_sample.xlsx
+++ b/Data/house_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\python_for_data_science\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\python_for_data_science\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="138">
   <si>
     <t>产权性质</t>
   </si>
@@ -411,6 +411,33 @@
   </si>
   <si>
     <t>西元2017年4月21日</t>
+  </si>
+  <si>
+    <t>装修</t>
+  </si>
+  <si>
+    <t>豪华装修</t>
+  </si>
+  <si>
+    <t>精装修</t>
+  </si>
+  <si>
+    <t>简装修</t>
+  </si>
+  <si>
+    <t>中装修</t>
+  </si>
+  <si>
+    <t>楼层</t>
+  </si>
+  <si>
+    <t>低层</t>
+  </si>
+  <si>
+    <t>中层</t>
+  </si>
+  <si>
+    <t>高层</t>
   </si>
 </sst>
 </file>
@@ -814,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -830,7 +857,7 @@
     <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>116</v>
       </c>
@@ -858,8 +885,14 @@
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -890,8 +923,14 @@
       <c r="J2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -922,8 +961,14 @@
       <c r="J3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -954,8 +999,14 @@
       <c r="J4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>131</v>
+      </c>
+      <c r="L4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -986,8 +1037,14 @@
       <c r="J5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>132</v>
+      </c>
+      <c r="L5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1018,8 +1075,14 @@
       <c r="J6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1050,8 +1113,14 @@
       <c r="J7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1082,8 +1151,14 @@
       <c r="J8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1114,8 +1189,14 @@
       <c r="J9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>132</v>
+      </c>
+      <c r="L9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1146,8 +1227,14 @@
       <c r="J10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1178,8 +1265,14 @@
       <c r="J11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>132</v>
+      </c>
+      <c r="L11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1210,8 +1303,14 @@
       <c r="J12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1242,8 +1341,14 @@
       <c r="J13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>132</v>
+      </c>
+      <c r="L13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1274,8 +1379,14 @@
       <c r="J14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>132</v>
+      </c>
+      <c r="L14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1306,8 +1417,14 @@
       <c r="J15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>132</v>
+      </c>
+      <c r="L15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1338,8 +1455,14 @@
       <c r="J16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1370,8 +1493,14 @@
       <c r="J17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>131</v>
+      </c>
+      <c r="L17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1402,8 +1531,14 @@
       <c r="J18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>131</v>
+      </c>
+      <c r="L18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1434,8 +1569,14 @@
       <c r="J19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>132</v>
+      </c>
+      <c r="L19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1466,8 +1607,14 @@
       <c r="J20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1498,8 +1645,14 @@
       <c r="J21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>132</v>
+      </c>
+      <c r="L21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1530,8 +1683,14 @@
       <c r="J22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1562,8 +1721,14 @@
       <c r="J23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>130</v>
+      </c>
+      <c r="L23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1594,8 +1759,14 @@
       <c r="J24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>131</v>
+      </c>
+      <c r="L24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1626,8 +1797,14 @@
       <c r="J25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>131</v>
+      </c>
+      <c r="L25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1658,8 +1835,14 @@
       <c r="J26" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>131</v>
+      </c>
+      <c r="L26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1690,8 +1873,14 @@
       <c r="J27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>131</v>
+      </c>
+      <c r="L27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1722,8 +1911,14 @@
       <c r="J28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>131</v>
+      </c>
+      <c r="L28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1754,8 +1949,14 @@
       <c r="J29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>131</v>
+      </c>
+      <c r="L29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1785,6 +1986,12 @@
       </c>
       <c r="J30" t="s">
         <v>6</v>
+      </c>
+      <c r="K30" t="s">
+        <v>131</v>
+      </c>
+      <c r="L30" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>